<commit_message>
adicionando seção de estudo de projetos
</commit_message>
<xml_diff>
--- a/banco_controle_de_atrasos.xlsx
+++ b/banco_controle_de_atrasos.xlsx
@@ -368,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1028,7 +1028,7 @@
         <v>45419.22151988426</v>
       </c>
       <c r="M12">
-        <v>101.712928</v>
+        <v>116.802755</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1">
@@ -1226,7 +1226,7 @@
         <v>45432.97784560185</v>
       </c>
       <c r="M16">
-        <v>98.784479</v>
+        <v>113.874306</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1">
@@ -1782,7 +1782,7 @@
         <v>45467.93827454861</v>
       </c>
       <c r="M27">
-        <v>63.824051</v>
+        <v>78.913877</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="1">
@@ -1833,7 +1833,7 @@
         <v>45467.93916752315</v>
       </c>
       <c r="M28">
-        <v>63.823148</v>
+        <v>78.912975</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Execução</t>
+          <t>NPS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1943,8 +1943,11 @@
       <c r="K30" s="2">
         <v>45498.87956074074</v>
       </c>
+      <c r="L30" s="2">
+        <v>45534.89751761574</v>
+      </c>
       <c r="M30">
-        <v>32.88265</v>
+        <v>36.017836</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="1">
@@ -1955,7 +1958,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Execução</t>
+          <t>NPS</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1964,7 +1967,7 @@
         </is>
       </c>
       <c r="D31" s="2">
-        <v>45537.92663194444</v>
+        <v>45539.10416666667</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1997,14 +2000,17 @@
       <c r="K31" s="2">
         <v>45510.92804918981</v>
       </c>
+      <c r="L31" s="2">
+        <v>45538.94357984954</v>
+      </c>
       <c r="M31">
-        <v>20.834271</v>
+        <v>28.015521</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1">
       <c r="A32" t="inlineStr">
         <is>
-          <t>PF24037 - Marilia Matasha.</t>
+          <t>PF24037 - Marilia Matasha</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2049,7 +2055,7 @@
         <v>45524.85623391204</v>
       </c>
       <c r="M32">
-        <v>6.906088</v>
+        <v>21.995914</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
@@ -2060,7 +2066,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Forms de feedback</t>
+          <t>Finalizados™</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2160,7 +2166,7 @@
         <v>45519.5697700926</v>
       </c>
       <c r="M34">
-        <v>12.192546</v>
+        <v>27.282373</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
@@ -2211,7 +2217,7 @@
         <v>45519.68877888889</v>
       </c>
       <c r="M35">
-        <v>12.073542</v>
+        <v>27.163368</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1">
@@ -2257,7 +2263,7 @@
     <row r="37" ht="18" customHeight="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PF24044 - Marcus</t>
+          <t>PF24043 - Mario Andrade</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2267,51 +2273,51 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Consultoria estatística</t>
+          <t>Power BI</t>
         </is>
       </c>
       <c r="D37" s="2">
-        <v>45590.74818287037</v>
+        <v>45553.88295138889</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4 – Educação de qualidade</t>
+          <t>8 – Trabalho decente e crescimento econômico</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Gabriel Henrique Ovidio de Araújo</t>
+          <t>Ana Vasconcelos</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enrique Istvan, Gabriela Ludovico Cassimiro Coutinho </t>
+          <t xml:space="preserve">Ana beatriz de carvalho lopes </t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Iza Débora Santos</t>
+          <t>Marina Braulio</t>
         </is>
       </c>
       <c r="I37">
-        <v>1040</v>
+        <v>1000</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Exploratória, Métodos 2, Regressão</t>
+          <t>PowerBI</t>
         </is>
       </c>
       <c r="K37" s="2">
-        <v>45530.7473067824</v>
+        <v>45534.00668230324</v>
       </c>
       <c r="M37">
-        <v>1.015012</v>
+        <v>12.845463</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PF24045 - Bernardo</t>
+          <t>PF24044 - Marcus</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2321,51 +2327,51 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Exploratória, Métodos 2</t>
+          <t>Consultoria estatística</t>
         </is>
       </c>
       <c r="D38" s="2">
-        <v>45552.14604166667</v>
+        <v>45590.74818287037</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3 – Saúde e bem-estar</t>
+          <t>4 – Educação de qualidade</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>João Vitor Balbino</t>
+          <t>Gabriel Henrique Ovidio de Araújo</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Bernardo Suffert Monteiro, Felipe Baptista de Carvalho</t>
+          <t xml:space="preserve">Enrique Istvan, Gabriela Ludovico Cassimiro Coutinho </t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Isabela Yule</t>
+          <t>Iza Débora Santos</t>
         </is>
       </c>
       <c r="I38">
-        <v>2500</v>
+        <v>1040</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Métodos 2</t>
+          <t>Exploratória, Métodos 2, Regressão</t>
         </is>
       </c>
       <c r="K38" s="2">
-        <v>45530.14654862268</v>
+        <v>45530.7473067824</v>
       </c>
       <c r="M38">
-        <v>1.615775</v>
+        <v>16.104838</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PF24046 - Kamylla Xavier (Termo Aditivo)</t>
+          <t>PF24045 - Bernardo</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2375,128 +2381,156 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Consultoria estatística</t>
-        </is>
+          <t>Exploratória, Métodos 2</t>
+        </is>
+      </c>
+      <c r="D39" s="2">
+        <v>45552.14604166667</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4 – Educação de qualidade</t>
+          <t>3 – Saúde e bem-estar</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Ana Luisa Sousa de Oliveira</t>
+          <t>João Vitor Balbino</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Ana Luisa Sousa de Oliveira</t>
+          <t>Bernardo Suffert Monteiro, Felipe Baptista de Carvalho</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Ana Luisa Sousa de Oliveira</t>
+          <t>Isabela Yule</t>
         </is>
       </c>
       <c r="I39">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Exploratória</t>
+          <t>Métodos 2</t>
         </is>
       </c>
       <c r="K39" s="2">
-        <v>45527.08491319444</v>
+        <v>45530.14654862268</v>
       </c>
       <c r="M39">
-        <v>4.677407</v>
+        <v>16.705602</v>
       </c>
     </row>
     <row r="40" ht="18" customHeight="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PF24047 - Vivian Gregori</t>
+          <t>PF24046 - Kamylla Xavier (Termo Aditivo)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Caixa de entrada</t>
+          <t>Execução</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Consultoria estatística</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5 – Igualdade de gênero</t>
+          <t>4 – Educação de qualidade</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Lucas Fonseca Alves</t>
+          <t>Ana Luisa Sousa de Oliveira</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>André Costa</t>
+          <t>Ana Luisa Sousa de Oliveira</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Carlos César Yoshitake Júnior</t>
+          <t>Ana Luisa Sousa de Oliveira</t>
         </is>
       </c>
       <c r="I40">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Exploratória, Métodos 2</t>
-        </is>
+          <t>Exploratória</t>
+        </is>
+      </c>
+      <c r="K40" s="2">
+        <v>45527.08491319444</v>
+      </c>
+      <c r="M40">
+        <v>19.767234</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="1">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PF24048 - Tárcio Borborema</t>
+          <t>PF24047 - Vivian Gregori</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Caixa de entrada</t>
-        </is>
+          <t>Execução</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Exploratória, Métodos 2</t>
+        </is>
+      </c>
+      <c r="D41" s="2">
+        <v>45567.45509259259</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3 – Saúde e bem-estar</t>
+          <t>5 – Igualdade de gênero</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>João Vitor Neves da Costa</t>
+          <t>Lucas Fonseca Alves</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Felipe Adriano, Lucas Caires de Sousa</t>
+          <t>André Costa</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Nathália Lobo</t>
+          <t>Carlos César Yoshitake Júnior</t>
         </is>
       </c>
       <c r="I41">
-        <v>2580</v>
+        <v>4000</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
           <t>Exploratória, Métodos 2</t>
         </is>
+      </c>
+      <c r="K41" s="2">
+        <v>45539.44600791667</v>
+      </c>
+      <c r="M41">
+        <v>7.406134</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PJ23036 - Imuna Balística</t>
+          <t>PF24048 - Tárcio Borborema</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2504,48 +2538,53 @@
           <t>Execução</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Exploratória, Métodos 2</t>
+        </is>
+      </c>
       <c r="D42" s="2">
-        <v>45440.92446759259</v>
+        <v>45548.9325</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>8 – Trabalho decente e crescimento econômico</t>
+          <t>3 – Saúde e bem-estar</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Vítor Hott Amorim</t>
+          <t>João Vitor Neves da Costa</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Rafaela Leitao</t>
+          <t>Felipe Adriano, Lucas Caires de Sousa</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Hugo de Lima Saigg</t>
+          <t>Nathália Lobo</t>
         </is>
       </c>
       <c r="I42">
-        <v>2000</v>
+        <v>2580</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Datastudio</t>
+          <t>Exploratória, Métodos 2</t>
         </is>
       </c>
       <c r="K42" s="2">
-        <v>45427.55216987268</v>
+        <v>45531.93302607638</v>
       </c>
       <c r="M42">
-        <v>104.21015</v>
+        <v>14.91912</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PJ24002 - Brickell Estates</t>
+          <t>PF24050 - Luís Pinheiro</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2555,22 +2594,25 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Power BI</t>
-        </is>
+          <t>Coleta de dados, Questionário</t>
+        </is>
+      </c>
+      <c r="D43" s="2">
+        <v>45544.44565972222</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>9 – Indústria, inovação e infraestrutura</t>
+          <t>8 – Trabalho decente e crescimento econômico</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Marina Gabriela de Oliveira Cadete, Nathália Lobo</t>
+          <t>Lucas Fonseca Alves</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Felipe Adriano, Gabriela Ludovico Cassimiro Coutinho </t>
+          <t>Felipe Adriano</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2579,106 +2621,90 @@
         </is>
       </c>
       <c r="I43">
-        <v>8000</v>
+        <v>2673</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>PowerBI</t>
+          <t>Coleta de Dados, Questionários</t>
         </is>
       </c>
       <c r="K43" s="2">
-        <v>45328.70732599538</v>
+        <v>45539.44592302083</v>
       </c>
       <c r="L43" s="2">
-        <v>45401.8897403588</v>
+        <v>45539.44607392361</v>
       </c>
       <c r="M43">
-        <v>73.182407</v>
+        <v>0.00015</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>PJ24009 - Juveniz Jr.</t>
+          <t>PF24051 - Ana Paula</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Finalizados™</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Consultoria estatística, Power BI</t>
+          <t>Caixa de entrada</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>8 – Trabalho decente e crescimento econômico</t>
+          <t>3 – Saúde e bem-estar</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Marina Gabriela de Oliveira Cadete</t>
+          <t>Elisa Amaral Santos</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Gabriel Leonardo Fadul, Heitor Roncato de Souza</t>
+          <t>Humberto Amorim, Lucas Caires de Sousa</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Iza Débora Santos</t>
+          <t>Nathália Lobo</t>
         </is>
       </c>
       <c r="I44">
-        <v>1620</v>
+        <v>1500</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Consultoria estatística, PowerBI</t>
-        </is>
-      </c>
-      <c r="K44" s="2">
-        <v>45385.13827570602</v>
-      </c>
-      <c r="L44" s="2">
-        <v>45416.59761787037</v>
-      </c>
-      <c r="M44">
-        <v>31.45934</v>
+          <t>Exploratória, Métodos 2</t>
+        </is>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>PJ24010 - Fernanda Gonçalves</t>
+          <t>PJ23036 - Imuna Balística</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>NPS</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Exploratória</t>
-        </is>
+          <t>Execução</t>
+        </is>
+      </c>
+      <c r="D45" s="2">
+        <v>45440.92446759259</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3 – Saúde e bem-estar</t>
+          <t>8 – Trabalho decente e crescimento econômico</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Nathália Lobo</t>
+          <t>Vítor Hott Amorim</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Felipe Adriano, Humberto Amorim</t>
+          <t>Rafaela Leitao</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2687,32 +2713,29 @@
         </is>
       </c>
       <c r="I45">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Exploratória</t>
+          <t>Datastudio</t>
         </is>
       </c>
       <c r="K45" s="2">
-        <v>45390.51185645834</v>
-      </c>
-      <c r="L45" s="2">
-        <v>45432.97903460648</v>
+        <v>45427.55216987268</v>
       </c>
       <c r="M45">
-        <v>42.467176</v>
+        <v>119.299977</v>
       </c>
     </row>
     <row r="46" ht="18" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>PJ24011 - Urias Comércio de Autopeças</t>
+          <t>PJ24002 - Brickell Estates</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Fase de espera</t>
+          <t>Finalizados™</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2722,42 +2745,56 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>8 – Trabalho decente e crescimento econômico</t>
+          <t>9 – Indústria, inovação e infraestrutura</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Natasha Nuto Smidt</t>
+          <t>Marina Gabriela de Oliveira Cadete, Nathália Lobo</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Rafaela Leitao</t>
+          <t xml:space="preserve">Felipe Adriano, Gabriela Ludovico Cassimiro Coutinho </t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Breno Sanchi Cardoso do Amaral</t>
+          <t>Iza Débora Santos</t>
         </is>
       </c>
       <c r="I46">
-        <v>3846</v>
+        <v>8000</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
           <t>PowerBI</t>
         </is>
+      </c>
+      <c r="K46" s="2">
+        <v>45328.70732599538</v>
+      </c>
+      <c r="L46" s="2">
+        <v>45401.8897403588</v>
+      </c>
+      <c r="M46">
+        <v>73.182407</v>
       </c>
     </row>
     <row r="47" ht="18" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>PJ24019 - Carneiros Temporada Viagens e Turismo Ltda.</t>
+          <t>PJ24009 - Juveniz Jr.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Execução</t>
+          <t>Finalizados™</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Consultoria estatística, Power BI</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2767,66 +2804,66 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Júlia Lima Nosralla</t>
+          <t>Marina Gabriela de Oliveira Cadete</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Rafaela Leitao</t>
+          <t>Gabriel Leonardo Fadul, Heitor Roncato de Souza</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Marina Braulio</t>
+          <t>Iza Débora Santos</t>
         </is>
       </c>
       <c r="I47">
-        <v>3000</v>
+        <v>1620</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>PowerBI</t>
+          <t>Consultoria estatística, PowerBI</t>
         </is>
       </c>
       <c r="K47" s="2">
-        <v>45432.97918827547</v>
+        <v>45385.13827570602</v>
+      </c>
+      <c r="L47" s="2">
+        <v>45416.59761787037</v>
       </c>
       <c r="M47">
-        <v>98.783137</v>
+        <v>31.45934</v>
       </c>
     </row>
     <row r="48" ht="18" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PJ24028 - Marcos Rogério</t>
+          <t>PJ24010 - Fernanda Gonçalves</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Caixa de entrada</t>
+          <t>NPS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Power BI</t>
-        </is>
-      </c>
-      <c r="D48" s="2">
-        <v>45541.98517361112</v>
+          <t>Exploratória</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>16 – Paz, justiça e instituições eficazes</t>
+          <t>3 – Saúde e bem-estar</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Letícia Inacio Rodrigues de Lima</t>
+          <t>Nathália Lobo</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Gabriel Leonardo Fadul</t>
+          <t>Felipe Adriano, Humberto Amorim</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2835,27 +2872,27 @@
         </is>
       </c>
       <c r="I48">
-        <v>3105</v>
+        <v>1000</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Exploratória, PowerBI</t>
+          <t>Exploratória</t>
         </is>
       </c>
       <c r="K48" s="2">
-        <v>45503.98290200232</v>
+        <v>45390.51185645834</v>
       </c>
       <c r="L48" s="2">
-        <v>45511.88380702546</v>
+        <v>45432.97903460648</v>
       </c>
       <c r="M48">
-        <v>7.900903</v>
+        <v>42.467176</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>PJ24034 - Mercado Cultural</t>
+          <t>PJ24011 - Urias Comércio de Autopeças</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2865,25 +2902,22 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Exploratória</t>
-        </is>
-      </c>
-      <c r="D49" s="2">
-        <v>45517.66681712963</v>
+          <t>Power BI</t>
+        </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4 – Educação de qualidade</t>
+          <t>8 – Trabalho decente e crescimento econômico</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>João Vitor Balbino</t>
+          <t>Natasha Nuto Smidt</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Heitor Roncato de Souza</t>
+          <t>Rafaela Leitao</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2892,27 +2926,18 @@
         </is>
       </c>
       <c r="I49">
-        <v>1500</v>
+        <v>3846</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Amostragem, Exploratória</t>
-        </is>
-      </c>
-      <c r="K49" s="2">
-        <v>45511.0478681713</v>
-      </c>
-      <c r="L49" s="2">
-        <v>45518.79784585648</v>
-      </c>
-      <c r="M49">
-        <v>7.749977</v>
+          <t>PowerBI</t>
+        </is>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PJ24041 - Romeu</t>
+          <t>PJ24019 - Carneiros Temporada Viagens e Turismo Ltda.</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2920,36 +2945,28 @@
           <t>Execução</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Power BI</t>
-        </is>
-      </c>
-      <c r="D50" s="2">
-        <v>45544.03097222222</v>
-      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>3 – Saúde e bem-estar</t>
+          <t>8 – Trabalho decente e crescimento econômico</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Murilo Massaro</t>
+          <t>Júlia Lima Nosralla</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Bernardo Suffert Monteiro, Gabriel Leonardo Fadul</t>
+          <t>Rafaela Leitao</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Lavínia Vieira Bueno</t>
+          <t>Marina Braulio</t>
         </is>
       </c>
       <c r="I50">
-        <v>2360</v>
+        <v>3000</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -2957,21 +2974,21 @@
         </is>
       </c>
       <c r="K50" s="2">
-        <v>45527.78959439815</v>
+        <v>45432.97918827547</v>
       </c>
       <c r="M50">
-        <v>3.972731</v>
+        <v>113.872963</v>
       </c>
     </row>
     <row r="51" ht="18" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PJ24049- Parolle</t>
+          <t>PJ24028 - Marcos Rogério</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Execução</t>
+          <t>Caixa de entrada</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2980,92 +2997,263 @@
         </is>
       </c>
       <c r="D51" s="2">
-        <v>45555.57207175926</v>
+        <v>45541.98517361112</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>8 – Trabalho decente e crescimento econômico</t>
+          <t>16 – Paz, justiça e instituições eficazes</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Marina Gabriela de Oliveira Cadete</t>
+          <t>Letícia Inacio Rodrigues de Lima</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gabriela Ludovico Cassimiro Coutinho </t>
+          <t>Gabriel Leonardo Fadul</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Luísa Ulhoa Chaves Padula</t>
+          <t>Hugo de Lima Saigg</t>
         </is>
       </c>
       <c r="I51">
-        <v>8700</v>
+        <v>3105</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>PowerBI</t>
+          <t>Exploratória, PowerBI</t>
         </is>
       </c>
       <c r="K51" s="2">
-        <v>45530.67649201389</v>
+        <v>45503.98290200232</v>
+      </c>
+      <c r="L51" s="2">
+        <v>45511.88380702546</v>
       </c>
       <c r="M51">
-        <v>1.085833</v>
+        <v>7.900903</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
+          <t>PJ24034 - Mercado Cultural</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Fase de espera</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Exploratória</t>
+        </is>
+      </c>
+      <c r="D52" s="2">
+        <v>45517.66681712963</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>4 – Educação de qualidade</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>João Vitor Balbino</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Heitor Roncato de Souza</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Breno Sanchi Cardoso do Amaral</t>
+        </is>
+      </c>
+      <c r="I52">
+        <v>1500</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Amostragem, Exploratória</t>
+        </is>
+      </c>
+      <c r="K52" s="2">
+        <v>45511.0478681713</v>
+      </c>
+      <c r="L52" s="2">
+        <v>45518.79784585648</v>
+      </c>
+      <c r="M52">
+        <v>7.749977</v>
+      </c>
+    </row>
+    <row r="53" ht="18" customHeight="1">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>PJ24041 - Romeu</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>NPS</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Power BI</t>
+        </is>
+      </c>
+      <c r="D53" s="2">
+        <v>45544.99930555555</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>3 – Saúde e bem-estar</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Murilo Massaro</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Bernardo Suffert Monteiro, Gabriel Leonardo Fadul</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Lavínia Vieira Bueno</t>
+        </is>
+      </c>
+      <c r="I53">
+        <v>2360</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>PowerBI</t>
+        </is>
+      </c>
+      <c r="K53" s="2">
+        <v>45527.78959439815</v>
+      </c>
+      <c r="L53" s="2">
+        <v>45544.92891146991</v>
+      </c>
+      <c r="M53">
+        <v>17.139306</v>
+      </c>
+    </row>
+    <row r="54" ht="18" customHeight="1">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>PJ24049 - Parolle</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Execução</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Power BI</t>
+        </is>
+      </c>
+      <c r="D54" s="2">
+        <v>45555.57207175926</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>8 – Trabalho decente e crescimento econômico</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Marina Gabriela de Oliveira Cadete</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gabriela Ludovico Cassimiro Coutinho </t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Luísa Ulhoa Chaves Padula</t>
+        </is>
+      </c>
+      <c r="I54">
+        <v>8700</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>PowerBI</t>
+        </is>
+      </c>
+      <c r="K54" s="2">
+        <v>45530.67649201389</v>
+      </c>
+      <c r="M54">
+        <v>16.17566</v>
+      </c>
+    </row>
+    <row r="55" ht="18" customHeight="1">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>Secovi Janeiro</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B55" t="inlineStr">
         <is>
           <t>Finalizados™</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>Python, Scrapping</t>
         </is>
       </c>
-      <c r="D52" s="2">
+      <c r="D55" s="2">
         <v>45320</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t>Pedro Tepedino, Stefan Zurman Gonçalves, Vítor Hott Amorim</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G55" t="inlineStr">
         <is>
           <t>Stefan Zurman Gonçalves</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t>Stefan Zurman Gonçalves</t>
         </is>
       </c>
-      <c r="I52">
+      <c r="I55">
         <v>800</v>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="J55" t="inlineStr">
         <is>
           <t>Python, Scrapping</t>
         </is>
       </c>
-      <c r="K52" s="2">
+      <c r="K55" s="2">
         <v>45309.60219337963</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L55" s="2">
         <v>45368.55699078704</v>
       </c>
-      <c r="M52">
+      <c r="M55">
         <v>14.292072</v>
       </c>
     </row>

</xml_diff>